<commit_message>
correcciones en excel con datos de rendimiento
</commit_message>
<xml_diff>
--- a/Docs/Comparación-rendimiento-r1-r2.xlsx
+++ b/Docs/Comparación-rendimiento-r1-r2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanc\OneDrive\Documentos\repos\EDA\Reto2-G06\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dbc1bd32c169fa06/Documentos/repos/EDA/Reto2-G06/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F97D327-013A-4C3B-B1CA-5085243CEFE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FDF2384-D008-4E90-A856-5572D42100CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{635EB517-7885-47A9-8218-4DDA237547AF}"/>
   </bookViews>

</xml_diff>